<commit_message>
start adding in asbuilt data
</commit_message>
<xml_diff>
--- a/data/exclusive_data_tier_2017-01-01_2025-01-01.xlsx
+++ b/data/exclusive_data_tier_2017-01-01_2025-01-01.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schellma/Dropbox/DUNE-computing/CCB-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{890642EB-018A-3C4D-8EB6-A90936C05ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD0885A-AF0A-B649-BB47-4F2C391BB67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16460"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exclusive_data_tier_2017-01-01_" sheetId="1" r:id="rId1"/>
@@ -154,13 +154,13 @@
     <t xml:space="preserve">  detector-simulated</t>
   </si>
   <si>
-    <t>X</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
@@ -999,11 +999,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1084,7 +1085,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1116,7 +1117,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1148,7 +1149,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1180,7 +1181,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1212,7 +1213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1244,7 +1245,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1276,7 +1277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1311,7 +1312,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1375,7 +1376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1407,7 +1408,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1439,7 +1440,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1471,7 +1472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1503,7 +1504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1535,7 +1536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1567,7 +1568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1599,7 +1600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1631,7 +1632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1663,7 +1664,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1695,7 +1696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1759,7 +1760,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1791,7 +1792,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1823,7 +1824,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1855,7 +1856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1887,7 +1888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1919,7 +1920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1951,7 +1952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -2047,7 +2048,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2079,7 +2080,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2143,7 +2144,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2175,7 +2176,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2207,7 +2208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2239,7 +2240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2271,7 +2272,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -2303,7 +2304,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -2335,7 +2336,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -2367,7 +2368,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2399,7 +2400,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>35</v>
       </c>
@@ -2431,7 +2432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>35</v>
       </c>
@@ -2463,7 +2464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -2495,7 +2496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -2527,7 +2528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -2559,7 +2560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -2591,7 +2592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -2623,7 +2624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -2655,7 +2656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -2687,7 +2688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -2719,7 +2720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -2751,7 +2752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -2783,7 +2784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>35</v>
       </c>
@@ -2815,7 +2816,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -2847,7 +2848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -2879,7 +2880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -2911,7 +2912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>35</v>
       </c>
@@ -2943,7 +2944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>35</v>
       </c>
@@ -2975,7 +2976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -3007,7 +3008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -3039,7 +3040,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -3071,7 +3072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>35</v>
       </c>
@@ -3103,7 +3104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -3135,7 +3136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>35</v>
       </c>
@@ -3168,7 +3169,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J67">
+  <autoFilter ref="A1:J67" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="detector-simulated"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J67">
       <sortCondition descending="1" ref="G1:G67"/>
     </sortState>

</xml_diff>

<commit_message>
add in a lot of osg reports
</commit_message>
<xml_diff>
--- a/data/exclusive_data_tier_2017-01-01_2025-01-01.xlsx
+++ b/data/exclusive_data_tier_2017-01-01_2025-01-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schellma/Dropbox/DUNE-computing/CCB-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD0885A-AF0A-B649-BB47-4F2C391BB67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD520DC-0961-BD4A-B2DF-EB54782DD1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1053,7 +1053,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -3170,14 +3170,16 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J67" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="detector"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="3">
       <filters>
-        <filter val="detector-simulated"/>
+        <filter val="raw"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J67">
-      <sortCondition descending="1" ref="G1:G67"/>
-    </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>